<commit_message>
Fixed the neural network. High test error of 0.05
</commit_message>
<xml_diff>
--- a/FinalProject/Q2/regression_results.xlsx
+++ b/FinalProject/Q2/regression_results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t xml:space="preserve">Technique</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t xml:space="preserve">Random forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neural Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_it = 1000, learning_rate = 0.0001</t>
   </si>
 </sst>
 </file>
@@ -145,16 +151,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16:D16"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.94"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -211,6 +217,17 @@
       </c>
       <c r="C5" s="0" t="n">
         <v>0.0119697</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.050206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented k-nearest neighbours with hyperparameter (number of neighbours) tuning
</commit_message>
<xml_diff>
--- a/FinalProject/Q2/regression_results.xlsx
+++ b/FinalProject/Q2/regression_results.xlsx
@@ -20,15 +20,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t xml:space="preserve">Technique</t>
   </si>
   <si>
+    <t xml:space="preserve">Training error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test error</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hyperparameters</t>
   </si>
   <si>
-    <t xml:space="preserve">Test error</t>
+    <t xml:space="preserve">Linear regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ridge regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alpha = 0.014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lasso regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alpha = 8.7*10^-7</t>
   </si>
   <si>
     <t xml:space="preserve">Extra trees</t>
@@ -55,7 +73,37 @@
     <t xml:space="preserve">Neural Network</t>
   </si>
   <si>
-    <t xml:space="preserve">n_it = 1000, learning_rate = 0.0001</t>
+    <t xml:space="preserve">n_it = 1000, learning_rate = 0.0001, layer_dims = [5, 8, 6, 1], tanh * 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_it = 2500, learning_rate = 0.0001, layer_dims = [5, 8, 6, 1], tanh * 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_it = 2500, learning_rate = 0.0001, layer_dims = [5, 8, 6, 3, 1], tanh * 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SVM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kernel = rbf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kernel = linear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epsilon = 0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epsilon = 0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearest Neighbours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_neighbours = 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_neighbours = 3</t>
   </si>
 </sst>
 </file>
@@ -70,6 +118,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -151,17 +200,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.8"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="61.38"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -174,60 +224,201 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="B2" s="0" t="n">
+        <v>0.0145589</v>
+      </c>
       <c r="C2" s="0" t="n">
-        <v>0.0119574</v>
+        <v>0.0146015</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="0" t="n">
+        <v>0.0145587</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.014602</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>0.0119401</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="0" t="n">
+        <v>0.0145586</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.0146029</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>0.0242965</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>6</v>
-      </c>
       <c r="C5" s="0" t="n">
-        <v>0.0119697</v>
+        <v>0.0119574</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.0119401</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.0242965</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.0119697</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.050206</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.0498693</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.0498685</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.0157858</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.016758</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.0132151</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.0117536</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.0119018</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>0.050206</v>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.012488</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.0137314</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>